<commit_message>
initial commit on internals
</commit_message>
<xml_diff>
--- a/A2_Booking_Parameters.xlsx
+++ b/A2_Booking_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\A2_Tickets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtm3004\Documents\Python Scripts\A2_Tickets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01FDC99-2BC5-4AF9-AADF-673C819DD745}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E0C98-1DC9-457A-A3EE-19A048FCEA3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DFD53A3-49CE-4847-B52F-30E2D27F0F4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{2DFD53A3-49CE-4847-B52F-30E2D27F0F4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Banks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Int Port" sheetId="4" r:id="rId4"/>
     <sheet name="Unexcor_Codes" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -502,8 +502,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,125 +824,125 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -957,7 +960,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,8 +1391,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>